<commit_message>
previo vs criterio 2
</commit_message>
<xml_diff>
--- a/Docs importantes/previoVSCriterio1.xlsx
+++ b/Docs importantes/previoVSCriterio1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Investigacion-maxima-diversidad\Docs importantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{959B7976-14E7-4BAE-84D9-FED6BF38E485}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9279B6F-DB2F-433B-9CB9-71DEA868E714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{624528B1-719E-46FD-9C2E-53A661800D81}"/>
   </bookViews>
@@ -185,7 +185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -218,7 +218,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,17 +536,17 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -578,31 +578,31 @@
       </c>
       <c r="B2" s="1">
         <f>AVERAGE(B9:B32)</f>
-        <v>6.2333864965443868E-3</v>
+        <v>0.3994002702090933</v>
       </c>
       <c r="C2" s="1">
         <f t="shared" ref="C2:H2" si="0">AVERAGE(C9:C32)</f>
-        <v>0.33502462227918128</v>
+        <v>0.2284173864162358</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" si="0"/>
-        <v>4.8650160848652389E-2</v>
+        <v>0.32336207577119225</v>
       </c>
       <c r="E2" s="1">
         <f t="shared" si="0"/>
-        <v>10407.587234903556</v>
+        <v>12979.49687312662</v>
       </c>
       <c r="F2" s="1">
         <f t="shared" si="0"/>
-        <v>21.916666666666668</v>
+        <v>13.916666666666666</v>
       </c>
       <c r="G2" s="1">
         <f t="shared" si="0"/>
-        <v>0.9751646117621221</v>
+        <v>0.98023388104574138</v>
       </c>
       <c r="H2" s="1">
         <f t="shared" si="0"/>
-        <v>438.08371248743742</v>
+        <v>476.09236606867012</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -611,31 +611,31 @@
       </c>
       <c r="B3" s="1">
         <f>AVERAGE(I9:I32)</f>
-        <v>0.74140886287625418</v>
+        <v>0.13278809225856661</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:H3" si="1">AVERAGE(J9:J32)</f>
-        <v>8.9198395112649719E-3</v>
+        <v>0.31985329090652709</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" si="1"/>
-        <v>1.254350678218185</v>
+        <v>0.34883408695849161</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" si="1"/>
-        <v>18484.357853607082</v>
+        <v>3838.6618160559738</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" si="1"/>
-        <v>6.458333333333333</v>
+        <v>92.333333333333329</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" si="1"/>
-        <v>0.98280709582445647</v>
+        <v>0.97744691276959672</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" si="1"/>
-        <v>624.83301278001522</v>
+        <v>366.24466435571435</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -693,43 +693,43 @@
         <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>0.46102688533642799</v>
+        <v>0.65353693882200004</v>
       </c>
       <c r="D9" s="1">
-        <v>0.147682641682987</v>
+        <v>4.6406355537194299E-2</v>
       </c>
       <c r="E9" s="1">
-        <v>889.73028112378199</v>
+        <v>962.60261016029494</v>
       </c>
       <c r="F9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" s="1">
-        <v>0.98980230771555799</v>
+        <v>0.98853644387487904</v>
       </c>
       <c r="H9" s="1">
-        <v>142.60414916903099</v>
+        <v>143.622872676317</v>
       </c>
       <c r="I9" s="1">
-        <v>0.25</v>
+        <v>0.22222222222222199</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
+        <v>0.67802839154114103</v>
       </c>
       <c r="K9" s="1">
-        <v>0.78792176279301995</v>
+        <v>7.5930694354298101E-7</v>
       </c>
       <c r="L9" s="1">
-        <v>1254.9946511386199</v>
+        <v>833.16302723896604</v>
       </c>
       <c r="M9" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="N9" s="1">
-        <v>0.99226227852471205</v>
+        <v>0.98750762069683096</v>
       </c>
       <c r="O9" s="1">
-        <v>148.506864658479</v>
+        <v>142.625979762561</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -737,46 +737,46 @@
         <v>18</v>
       </c>
       <c r="B10" s="1">
-        <v>6.6666666666666596E-2</v>
+        <v>0.35294117647058798</v>
       </c>
       <c r="C10" s="1">
-        <v>0.48916461562048502</v>
+        <v>0.21665925651937801</v>
       </c>
       <c r="D10" s="1">
-        <v>0.108650106901197</v>
+        <v>0.30557399607928998</v>
       </c>
       <c r="E10" s="1">
-        <v>157.662934510165</v>
+        <v>212.024435464752</v>
       </c>
       <c r="F10" s="1">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="G10" s="1">
-        <v>0.91260715485962696</v>
+        <v>0.93065382856898704</v>
       </c>
       <c r="H10" s="1">
-        <v>94.262578718878601</v>
+        <v>108.131303612115</v>
       </c>
       <c r="I10" s="1">
-        <v>0.5</v>
+        <v>0.14285714285714199</v>
       </c>
       <c r="J10" s="1">
-        <v>1.70384756992858E-2</v>
+        <v>0.27153699438208501</v>
       </c>
       <c r="K10" s="1">
-        <v>0.77070607432245097</v>
+        <v>0.103475803033494</v>
       </c>
       <c r="L10" s="1">
-        <v>276.10828858208401</v>
+        <v>190.46053266458699</v>
       </c>
       <c r="M10" s="1">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="N10" s="1">
-        <v>0.93581500347615398</v>
+        <v>0.93776662151080104</v>
       </c>
       <c r="O10" s="1">
-        <v>97.905571022520306</v>
+        <v>102.85869977602999</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -784,46 +784,46 @@
         <v>19</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="C11" s="1">
-        <v>0.27993943389516801</v>
+        <v>0.100730982836855</v>
       </c>
       <c r="D11" s="1">
-        <v>6.4448261574462096E-2</v>
+        <v>0.27670309363691797</v>
       </c>
       <c r="E11" s="1">
-        <v>3281.9371280862501</v>
+        <v>3970.47351305452</v>
       </c>
       <c r="F11" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G11" s="1">
-        <v>0.99710873419437995</v>
+        <v>0.99957493319148305</v>
       </c>
       <c r="H11" s="1">
-        <v>279.88918125342701</v>
+        <v>279.90212593810497</v>
       </c>
       <c r="I11" s="1">
-        <v>0</v>
+        <v>0.30769230769230699</v>
       </c>
       <c r="J11" s="1">
-        <v>0</v>
+        <v>0.11834354121641</v>
       </c>
       <c r="K11" s="1">
-        <v>1</v>
+        <v>0.64954969644671801</v>
       </c>
       <c r="L11" s="1">
-        <v>13061.525987372501</v>
+        <v>3641.1702369207401</v>
       </c>
       <c r="M11" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="N11" s="1">
-        <v>1</v>
+        <v>0.995680402772397</v>
       </c>
       <c r="O11" s="1">
-        <v>397.12549043918199</v>
+        <v>299.60444638743598</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -831,46 +831,46 @@
         <v>20</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="C12" s="1">
-        <v>0.23659890190669999</v>
+        <v>0.20730507138601401</v>
       </c>
       <c r="D12" s="1">
-        <v>0.21066638449950501</v>
+        <v>0.28240338429797701</v>
       </c>
       <c r="E12" s="1">
-        <v>484.06474141383597</v>
+        <v>515.14115508283101</v>
       </c>
       <c r="F12" s="1">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G12" s="1">
-        <v>0.94962358245853495</v>
+        <v>0.95523900482629698</v>
       </c>
       <c r="H12" s="1">
-        <v>166.36868427166101</v>
+        <v>170.105902680171</v>
       </c>
       <c r="I12" s="1">
-        <v>0.4</v>
+        <v>2.3255813953488299E-2</v>
       </c>
       <c r="J12" s="1">
-        <v>2.93741747011114E-3</v>
+        <v>0.43719976411553202</v>
       </c>
       <c r="K12" s="1">
-        <v>0.90907994349708399</v>
+        <v>0.20339121711522601</v>
       </c>
       <c r="L12" s="1">
-        <v>1183.62505831919</v>
+        <v>479.875284861475</v>
       </c>
       <c r="M12" s="1">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="N12" s="1">
-        <v>0.988096378802646</v>
+        <v>0.94922707840521503</v>
       </c>
       <c r="O12" s="1">
-        <v>163.820183125661</v>
+        <v>173.58815907124799</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -878,46 +878,46 @@
         <v>21</v>
       </c>
       <c r="B13" s="1">
-        <v>5.2631578947368397E-2</v>
+        <v>0.77272727272727204</v>
       </c>
       <c r="C13" s="1">
-        <v>0.75834534918909202</v>
+        <v>0.30290809276808101</v>
       </c>
       <c r="D13" s="1">
-        <v>5.2378757354256997E-2</v>
+        <v>0.328204606125722</v>
       </c>
       <c r="E13" s="1">
-        <v>1727.6249439278499</v>
+        <v>1617.64666004843</v>
       </c>
       <c r="F13" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G13" s="1">
-        <v>0.97555704257866904</v>
+        <v>0.98413427349305704</v>
       </c>
       <c r="H13" s="1">
-        <v>207.611182728741</v>
+        <v>203.03499355052099</v>
       </c>
       <c r="I13" s="1">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J13" s="1">
-        <v>6.1300023510164101E-2</v>
+        <v>0.64058936487112095</v>
       </c>
       <c r="K13" s="1">
-        <v>0.702594807465172</v>
+        <v>0.11421184021909001</v>
       </c>
       <c r="L13" s="1">
-        <v>3553.3895450452701</v>
+        <v>1684.1164283749199</v>
       </c>
       <c r="M13" s="1">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="N13" s="1">
-        <v>0.99786465376643696</v>
+        <v>0.99077875838997898</v>
       </c>
       <c r="O13" s="1">
-        <v>211.30949176815901</v>
+        <v>194.79171795760899</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -925,46 +925,46 @@
         <v>22</v>
       </c>
       <c r="B14" s="1">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.28932023401659202</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.32932649419805599</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2385.8448455731</v>
+      </c>
+      <c r="F14" s="1">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.986893031042681</v>
+      </c>
+      <c r="H14" s="1">
+        <v>189.39163129955301</v>
+      </c>
+      <c r="I14" s="1">
         <v>0</v>
       </c>
-      <c r="C14" s="1">
-        <v>0.63449272805057</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2.49567407894834E-2</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1958.3428198566901</v>
-      </c>
-      <c r="F14" s="1">
-        <v>21</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0.99432563888133196</v>
-      </c>
-      <c r="H14" s="1">
-        <v>179.06756157022701</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0.75</v>
-      </c>
       <c r="J14" s="1">
-        <v>1.0587485434171401E-2</v>
+        <v>0.58336231752784395</v>
       </c>
       <c r="K14" s="1">
-        <v>0.71400574466810196</v>
+        <v>0.13694313930973201</v>
       </c>
       <c r="L14" s="1">
-        <v>4150.4219655625002</v>
+        <v>1360.45413539839</v>
       </c>
       <c r="M14" s="1">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="N14" s="1">
-        <v>0.985206570829818</v>
+        <v>0.98840833671471295</v>
       </c>
       <c r="O14" s="1">
-        <v>254.82402499185699</v>
+        <v>122.744546599557</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -972,46 +972,46 @@
         <v>23</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>0.11111111111111099</v>
       </c>
       <c r="C15" s="1">
-        <v>0.38365016130104801</v>
+        <v>0.21914855140977499</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>0.26647485672416099</v>
       </c>
       <c r="E15" s="1">
-        <v>6890.0377480199504</v>
+        <v>11274.4127620689</v>
       </c>
       <c r="F15" s="1">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="G15" s="1">
-        <v>0.997076269722589</v>
+        <v>0.99843529320124202</v>
       </c>
       <c r="H15" s="1">
-        <v>506.63723867339002</v>
+        <v>529.29634734676199</v>
       </c>
       <c r="I15" s="1">
-        <v>1</v>
+        <v>4.7619047619047603E-2</v>
       </c>
       <c r="J15" s="1">
-        <v>0</v>
+        <v>0.205237315105115</v>
       </c>
       <c r="K15" s="1">
-        <v>4.30496667064169</v>
+        <v>0.376253587017434</v>
       </c>
       <c r="L15" s="1">
-        <v>31803.1122999535</v>
+        <v>7371.0723802439497</v>
       </c>
       <c r="M15" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="N15" s="1">
-        <v>1</v>
+        <v>0.99683865016457196</v>
       </c>
       <c r="O15" s="1">
-        <v>796.25306548584399</v>
+        <v>510.94445920125003</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1022,43 +1022,43 @@
         <v>0</v>
       </c>
       <c r="C16" s="1">
-        <v>0.40419064850016001</v>
+        <v>0.32953185492728998</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>0.10387876420990701</v>
       </c>
       <c r="E16" s="1">
-        <v>159.52286911467201</v>
+        <v>189.497195414365</v>
       </c>
       <c r="F16" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G16" s="1">
-        <v>0.94316267164616596</v>
+        <v>0.94842359272482701</v>
       </c>
       <c r="H16" s="1">
-        <v>106.101550646047</v>
+        <v>106.053357701997</v>
       </c>
       <c r="I16" s="1">
-        <v>0.33333333333333298</v>
+        <v>0.375</v>
       </c>
       <c r="J16" s="1">
-        <v>7.8237293049224904E-4</v>
+        <v>0.330962365641228</v>
       </c>
       <c r="K16" s="1">
-        <v>0.940102585460447</v>
+        <v>4.12474684129224E-2</v>
       </c>
       <c r="L16" s="1">
-        <v>278.46820294412203</v>
+        <v>191.622406133542</v>
       </c>
       <c r="M16" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="N16" s="1">
-        <v>0.98283974962360898</v>
+        <v>0.95839546857335101</v>
       </c>
       <c r="O16" s="1">
-        <v>107.379024131321</v>
+        <v>106.053357455285</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1066,46 +1066,46 @@
         <v>25</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>0.68421052631578905</v>
       </c>
       <c r="C17" s="1">
-        <v>0.49130054921553101</v>
+        <v>0.30342276606801699</v>
       </c>
       <c r="D17" s="1">
-        <v>0.20241629596191801</v>
+        <v>0.26413517595938801</v>
       </c>
       <c r="E17" s="1">
-        <v>233.21870756328599</v>
+        <v>292.41606697299898</v>
       </c>
       <c r="F17" s="1">
+        <v>19</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.90992515272475105</v>
+      </c>
+      <c r="H17" s="1">
+        <v>105.046054427138</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.12903225806451599</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.57622900090431795</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.24493083532106599</v>
+      </c>
+      <c r="L17" s="1">
+        <v>243.352440780573</v>
+      </c>
+      <c r="M17" s="1">
         <v>31</v>
       </c>
-      <c r="G17" s="1">
-        <v>0.94329165530715597</v>
-      </c>
-      <c r="H17" s="1">
-        <v>100.61689416032399</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0.30769230769230699</v>
-      </c>
-      <c r="J17" s="1">
-        <v>3.58323336137015E-2</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0.60422311796172701</v>
-      </c>
-      <c r="L17" s="1">
-        <v>279.77184753665603</v>
-      </c>
-      <c r="M17" s="1">
-        <v>13</v>
-      </c>
       <c r="N17" s="1">
-        <v>0.95613860231650505</v>
+        <v>0.915921748945833</v>
       </c>
       <c r="O17" s="1">
-        <v>100.683499755559</v>
+        <v>100.515474296889</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1113,46 +1113,46 @@
         <v>26</v>
       </c>
       <c r="B18" s="1">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.111080033942922</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.29426856333137602</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1268.01743229263</v>
+      </c>
+      <c r="F18" s="1">
+        <v>28</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.96951029463619598</v>
+      </c>
+      <c r="H18" s="1">
+        <v>190.79706971952601</v>
+      </c>
+      <c r="I18" s="1">
         <v>0</v>
       </c>
-      <c r="C18" s="1">
-        <v>9.9484998802329097E-2</v>
-      </c>
-      <c r="D18" s="1">
-        <v>9.3116838707441002E-2</v>
-      </c>
-      <c r="E18" s="1">
-        <v>973.77227092543001</v>
-      </c>
-      <c r="F18" s="1">
-        <v>49</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0.959734744430082</v>
-      </c>
-      <c r="H18" s="1">
-        <v>190.67689098657701</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0.625</v>
-      </c>
       <c r="J18" s="1">
-        <v>1.7757185058947099E-2</v>
+        <v>0.22503198655671799</v>
       </c>
       <c r="K18" s="1">
-        <v>0.62087117766952304</v>
+        <v>0.363144010708703</v>
       </c>
       <c r="L18" s="1">
-        <v>2157.2867951110602</v>
+        <v>726.67532421894202</v>
       </c>
       <c r="M18" s="1">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="N18" s="1">
-        <v>0.97062681145909002</v>
+        <v>0.97906991060956705</v>
       </c>
       <c r="O18" s="1">
-        <v>250.06371259063999</v>
+        <v>149.08034176551701</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1160,46 +1160,46 @@
         <v>27</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
+        <v>0.58823529411764697</v>
       </c>
       <c r="C19" s="1">
-        <v>0.41095609603970901</v>
+        <v>0.354551960663054</v>
       </c>
       <c r="D19" s="1">
-        <v>2.63506716115227E-2</v>
+        <v>0.26604965996075802</v>
       </c>
       <c r="E19" s="1">
-        <v>1723.58170459388</v>
+        <v>2150.7218827040901</v>
       </c>
       <c r="F19" s="1">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G19" s="1">
-        <v>0.98777719684896104</v>
+        <v>0.98638201800923697</v>
       </c>
       <c r="H19" s="1">
-        <v>196.25748193345501</v>
+        <v>196.48760129381299</v>
       </c>
       <c r="I19" s="1">
-        <v>0.875</v>
+        <v>6.1224489795918297E-2</v>
       </c>
       <c r="J19" s="1">
-        <v>1.08341842915654E-2</v>
+        <v>0.57221956023042098</v>
       </c>
       <c r="K19" s="1">
-        <v>0.83630617445118505</v>
+        <v>0.14079821840264201</v>
       </c>
       <c r="L19" s="1">
-        <v>2861.9858401841102</v>
+        <v>1333.00115038533</v>
       </c>
       <c r="M19" s="1">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="N19" s="1">
-        <v>0.98822888214037896</v>
+        <v>0.97855226815327601</v>
       </c>
       <c r="O19" s="1">
-        <v>206.304881285497</v>
+        <v>195.23784549736399</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1207,46 +1207,46 @@
         <v>28</v>
       </c>
       <c r="B20" s="1">
-        <v>0</v>
+        <v>0.14285714285714199</v>
       </c>
       <c r="C20" s="1">
-        <v>0.31993119727638297</v>
+        <v>0.30731563229150699</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>0.32441930597789098</v>
       </c>
       <c r="E20" s="1">
-        <v>17134.452277815199</v>
+        <v>19693.302160515101</v>
       </c>
       <c r="F20" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G20" s="1">
-        <v>0.99679021212803098</v>
+        <v>1.00550145317527</v>
       </c>
       <c r="H20" s="1">
-        <v>540.77678436788904</v>
+        <v>540.89418522256005</v>
       </c>
       <c r="I20" s="1">
-        <v>1</v>
+        <v>0.25378787878787801</v>
       </c>
       <c r="J20" s="1">
-        <v>0</v>
+        <v>0.228613368884649</v>
       </c>
       <c r="K20" s="1">
-        <v>1.13298711911789</v>
+        <v>0.39572029906025802</v>
       </c>
       <c r="L20" s="1">
-        <v>19737.530618615001</v>
+        <v>3070.8592625852102</v>
       </c>
       <c r="M20" s="1">
-        <v>5</v>
+        <v>264</v>
       </c>
       <c r="N20" s="1">
-        <v>0.99019375341510096</v>
+        <v>0.966997401646157</v>
       </c>
       <c r="O20" s="1">
-        <v>1113.1671288028899</v>
+        <v>507.96966189504201</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1254,46 +1254,46 @@
         <v>29</v>
       </c>
       <c r="B21" s="1">
-        <v>3.03030303030303E-2</v>
+        <v>0.88</v>
       </c>
       <c r="C21" s="1">
-        <v>0.28401761914498802</v>
+        <v>5.7614274868164603E-2</v>
       </c>
       <c r="D21" s="1">
-        <v>0.122910265843751</v>
+        <v>0.51915122496811095</v>
       </c>
       <c r="E21" s="1">
-        <v>1121.00752678816</v>
+        <v>1294.5481275305201</v>
       </c>
       <c r="F21" s="1">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G21" s="1">
-        <v>0.94824237964459901</v>
+        <v>0.96081910632491296</v>
       </c>
       <c r="H21" s="1">
-        <v>146.36103160205599</v>
+        <v>178.025451783747</v>
       </c>
       <c r="I21" s="1">
-        <v>0.91304347826086896</v>
+        <v>0</v>
       </c>
       <c r="J21" s="1">
-        <v>1.34369439021249E-3</v>
+        <v>0.58235994923734602</v>
       </c>
       <c r="K21" s="1">
-        <v>0.786526177664717</v>
+        <v>4.8088763691489497E-2</v>
       </c>
       <c r="L21" s="1">
-        <v>1113.77333597442</v>
+        <v>1030.8018307899299</v>
       </c>
       <c r="M21" s="1">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="N21" s="1">
-        <v>0.974633771197572</v>
+        <v>0.98011311293693104</v>
       </c>
       <c r="O21" s="1">
-        <v>191.91039370844101</v>
+        <v>94.751255251661604</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1301,46 +1301,46 @@
         <v>30</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>0.78571428571428503</v>
       </c>
       <c r="C22" s="1">
-        <v>0.66438823325753904</v>
+        <v>0.42299639402649702</v>
       </c>
       <c r="D22" s="1">
-        <v>0</v>
+        <v>0.37840108765965902</v>
       </c>
       <c r="E22" s="1">
-        <v>37962.368610931298</v>
+        <v>32386.431437835701</v>
       </c>
       <c r="F22" s="1">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G22" s="1">
-        <v>0.99678438065207298</v>
+        <v>0.99752470372298097</v>
       </c>
       <c r="H22" s="1">
-        <v>643.89951138098399</v>
+        <v>643.97653401987998</v>
       </c>
       <c r="I22" s="1">
-        <v>1</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="J22" s="1">
-        <v>0</v>
+        <v>0.53125410447410804</v>
       </c>
       <c r="K22" s="1">
-        <v>1.5919158148718699</v>
+        <v>0.22232967063377601</v>
       </c>
       <c r="L22" s="1">
-        <v>111065.464532094</v>
+        <v>8809.0037762153206</v>
       </c>
       <c r="M22" s="1">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="N22" s="1">
-        <v>1</v>
+        <v>0.98800823427680295</v>
       </c>
       <c r="O22" s="1">
-        <v>1872.07604385234</v>
+        <v>595.84657147666599</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1348,46 +1348,46 @@
         <v>31</v>
       </c>
       <c r="B23" s="1">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.105787084311594</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.486721861837699</v>
+      </c>
+      <c r="E23" s="1">
+        <v>54186.859271806301</v>
+      </c>
+      <c r="F23" s="1">
+        <v>6</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.99523785983712898</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1044.8017522114501</v>
+      </c>
+      <c r="I23" s="1">
         <v>0</v>
       </c>
-      <c r="C23" s="1">
-        <v>0.28756880512254701</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
-        <v>33356.380586392297</v>
-      </c>
-      <c r="F23" s="1">
-        <v>15</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0.99055707536882998</v>
-      </c>
-      <c r="H23" s="1">
-        <v>1044.5695358134501</v>
-      </c>
-      <c r="I23" s="1">
-        <v>1</v>
-      </c>
       <c r="J23" s="1">
-        <v>0</v>
+        <v>0.305049673258322</v>
       </c>
       <c r="K23" s="1">
-        <v>2.6653758605513702</v>
+        <v>0.27661818529454502</v>
       </c>
       <c r="L23" s="1">
-        <v>59024.000351494498</v>
+        <v>12074.0034996705</v>
       </c>
       <c r="M23" s="1">
-        <v>4</v>
+        <v>123</v>
       </c>
       <c r="N23" s="1">
-        <v>0.99780533664176896</v>
+        <v>0.99513427588817405</v>
       </c>
       <c r="O23" s="1">
-        <v>1826.01717756825</v>
+        <v>782.80777996067002</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1395,46 +1395,46 @@
         <v>32</v>
       </c>
       <c r="B24" s="1">
-        <v>0</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="C24" s="1">
-        <v>0.54323376465923801</v>
+        <v>0.20451510505984499</v>
       </c>
       <c r="D24" s="1">
-        <v>0.10197695496235699</v>
+        <v>0.30056652893251801</v>
       </c>
       <c r="E24" s="1">
-        <v>620.80128505961602</v>
+        <v>1000.32131851656</v>
       </c>
       <c r="F24" s="1">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G24" s="1">
-        <v>0.96507227892323</v>
+        <v>0.98086693940111003</v>
       </c>
       <c r="H24" s="1">
-        <v>156.249470049801</v>
+        <v>160.33979118550201</v>
       </c>
       <c r="I24" s="1">
-        <v>0.66666666666666596</v>
+        <v>4.3478260869565202E-2</v>
       </c>
       <c r="J24" s="1">
-        <v>5.5617261269391399E-2</v>
+        <v>0.45721747458572698</v>
       </c>
       <c r="K24" s="1">
-        <v>0.59328698886616504</v>
+        <v>4.3932865738286898E-2</v>
       </c>
       <c r="L24" s="1">
-        <v>1019.1870230094</v>
+        <v>815.47564300558304</v>
       </c>
       <c r="M24" s="1">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N24" s="1">
-        <v>0.97412666783444102</v>
+        <v>0.982349215249815</v>
       </c>
       <c r="O24" s="1">
-        <v>166.691148998383</v>
+        <v>148.180048814065</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -1442,46 +1442,46 @@
         <v>33</v>
       </c>
       <c r="B25" s="1">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="C25" s="1">
-        <v>0.135117672209106</v>
+        <v>0.29689853033190899</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>0.266321060447963</v>
       </c>
       <c r="E25" s="1">
-        <v>5532.3697037072097</v>
+        <v>6413.2629755199596</v>
       </c>
       <c r="F25" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G25" s="1">
-        <v>1.00006252389949</v>
+        <v>1.00463507455102</v>
       </c>
       <c r="H25" s="1">
-        <v>71.263254727493404</v>
+        <v>95.183287877672996</v>
       </c>
       <c r="I25" s="1">
-        <v>1</v>
+        <v>0.53623188405797095</v>
       </c>
       <c r="J25" s="1">
-        <v>0</v>
+        <v>0.13985515103647</v>
       </c>
       <c r="K25" s="1">
-        <v>1.11081289818623</v>
+        <v>0.39744337908952798</v>
       </c>
       <c r="L25" s="1">
-        <v>4455.3862498629196</v>
+        <v>1048.0051746268</v>
       </c>
       <c r="M25" s="1">
-        <v>12</v>
+        <v>276</v>
       </c>
       <c r="N25" s="1">
-        <v>0.99594560502781904</v>
+        <v>0.97387136208579705</v>
       </c>
       <c r="O25" s="1">
-        <v>157.05005968654999</v>
+        <v>98.333950477986505</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1489,46 +1489,46 @@
         <v>34</v>
       </c>
       <c r="B26" s="1">
-        <v>0</v>
+        <v>0.28571428571428498</v>
       </c>
       <c r="C26" s="1">
-        <v>0.20062661779286101</v>
+        <v>0.204235710336997</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>0.44988117782481102</v>
       </c>
       <c r="E26" s="1">
-        <v>4593.9537287933999</v>
+        <v>4884.0866041077297</v>
       </c>
       <c r="F26" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G26" s="1">
-        <v>0.99651196730200298</v>
+        <v>1.0069808133159199</v>
       </c>
       <c r="H26" s="1">
-        <v>58.731079211294002</v>
+        <v>74.283551397548806</v>
       </c>
       <c r="I26" s="1">
-        <v>1</v>
+        <v>3.66300366300366E-3</v>
       </c>
       <c r="J26" s="1">
-        <v>0</v>
+        <v>0.28911005477032498</v>
       </c>
       <c r="K26" s="1">
-        <v>1.12030005869174</v>
+        <v>0.287152783794555</v>
       </c>
       <c r="L26" s="1">
-        <v>6343.5890340921196</v>
+        <v>1105.6699410731301</v>
       </c>
       <c r="M26" s="1">
-        <v>6</v>
+        <v>273</v>
       </c>
       <c r="N26" s="1">
-        <v>1.0008675637034099</v>
+        <v>0.98912115325857897</v>
       </c>
       <c r="O26" s="1">
-        <v>161.927222951766</v>
+        <v>81.008442047828098</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -1539,43 +1539,43 @@
         <v>0</v>
       </c>
       <c r="C27" s="1">
-        <v>2.6462667544703E-2</v>
+        <v>0.46458009488231999</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>0.16820018553802801</v>
       </c>
       <c r="E27" s="1">
-        <v>5095.5133028252303</v>
+        <v>6817.1321113011099</v>
       </c>
       <c r="F27" s="1">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G27" s="1">
-        <v>0.99722634485521</v>
+        <v>0.99995867551816597</v>
       </c>
       <c r="H27" s="1">
-        <v>74.806071190913798</v>
+        <v>77.494777612734197</v>
       </c>
       <c r="I27" s="1">
-        <v>1</v>
+        <v>0.778169014084507</v>
       </c>
       <c r="J27" s="1">
-        <v>0</v>
+        <v>0.119185113502979</v>
       </c>
       <c r="K27" s="1">
-        <v>2.38138448071801</v>
+        <v>0.43434310327605502</v>
       </c>
       <c r="L27" s="1">
-        <v>5951.6503175586704</v>
+        <v>1031.06379279354</v>
       </c>
       <c r="M27" s="1">
-        <v>7</v>
+        <v>284</v>
       </c>
       <c r="N27" s="1">
-        <v>0.99809012265061903</v>
+        <v>0.98284705579645903</v>
       </c>
       <c r="O27" s="1">
-        <v>166.249273348354</v>
+        <v>95.822676609787493</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -1583,46 +1583,46 @@
         <v>36</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="C28" s="1">
-        <v>0.21436432919611501</v>
+        <v>5.58032022635844E-2</v>
       </c>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>0.36319980000000002</v>
       </c>
       <c r="E28" s="1">
-        <v>1308.2979954707901</v>
+        <v>2043.1572166042499</v>
       </c>
       <c r="F28" s="1">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="G28" s="1">
-        <v>0.98375908368371601</v>
+        <v>1.0035544768176301</v>
       </c>
       <c r="H28" s="1">
-        <v>54.338525117944101</v>
+        <v>64.379159372171898</v>
       </c>
       <c r="I28" s="1">
-        <v>1</v>
+        <v>2.04081632653061E-2</v>
       </c>
       <c r="J28" s="1">
-        <v>2.2205234627019802E-12</v>
+        <v>8.3801764758208802E-2</v>
       </c>
       <c r="K28" s="1">
-        <v>0.974358974932095</v>
+        <v>0.71830985915492895</v>
       </c>
       <c r="L28" s="1">
-        <v>2158.9961635746499</v>
+        <v>697.12267081469304</v>
       </c>
       <c r="M28" s="1">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="N28" s="1">
-        <v>0.99618953432950996</v>
+        <v>0.98479177846614396</v>
       </c>
       <c r="O28" s="1">
-        <v>67.8108533043969</v>
+        <v>46.222919565332496</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -1630,46 +1630,46 @@
         <v>37</v>
       </c>
       <c r="B29" s="1">
-        <v>0</v>
+        <v>0.31578947368421001</v>
       </c>
       <c r="C29" s="1">
-        <v>0.13309221812036301</v>
+        <v>6.2952419424676706E-2</v>
       </c>
       <c r="D29" s="1">
-        <v>1.2049940478775899E-2</v>
+        <v>0.40202728512113201</v>
       </c>
       <c r="E29" s="1">
-        <v>124006.13827701</v>
+        <v>157167.72365000701</v>
       </c>
       <c r="F29" s="1">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="G29" s="1">
-        <v>0.99055822682086503</v>
+        <v>0.99370702920822496</v>
       </c>
       <c r="H29" s="1">
-        <v>5502.1285940768203</v>
+        <v>6270.8540588715596</v>
       </c>
       <c r="I29" s="1">
-        <v>0.92307692307692302</v>
+        <v>6.0606060606060601E-2</v>
       </c>
       <c r="J29" s="1">
-        <v>4.5714600096184702E-5</v>
+        <v>2.3849223847291101E-2</v>
       </c>
       <c r="K29" s="1">
-        <v>0.97222956814043304</v>
+        <v>0.84079926864307097</v>
       </c>
       <c r="L29" s="1">
-        <v>170608.004402141</v>
+        <v>43635.826557557499</v>
       </c>
       <c r="M29" s="1">
-        <v>13</v>
+        <v>231</v>
       </c>
       <c r="N29" s="1">
-        <v>0.99292746329583303</v>
+        <v>0.97380262605557699</v>
       </c>
       <c r="O29" s="1">
-        <v>6476.9794493497902</v>
+        <v>4199.8295762163098</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -1677,46 +1677,46 @@
         <v>38</v>
       </c>
       <c r="B30" s="1">
+        <v>0.77777777777777701</v>
+      </c>
+      <c r="C30" s="1">
+        <v>8.7276214833759604E-3</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.57647058823529396</v>
+      </c>
+      <c r="E30" s="1">
+        <v>198.65944050885</v>
+      </c>
+      <c r="F30" s="1">
+        <v>9</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.97705789418923805</v>
+      </c>
+      <c r="H30" s="1">
+        <v>16.589944773957601</v>
+      </c>
+      <c r="I30" s="1">
         <v>0</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0.15615705156521401</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1">
-        <v>127.702960130441</v>
-      </c>
-      <c r="F30" s="1">
-        <v>20</v>
-      </c>
-      <c r="G30" s="1">
-        <v>0.92736416933145505</v>
-      </c>
-      <c r="H30" s="1">
-        <v>13.4855565872806</v>
-      </c>
-      <c r="I30" s="1">
-        <v>1</v>
       </c>
       <c r="J30" s="1">
         <v>0</v>
       </c>
       <c r="K30" s="1">
-        <v>1.0194805194805101</v>
+        <v>1</v>
       </c>
       <c r="L30" s="1">
-        <v>476.28481029898597</v>
+        <v>197.65329741494099</v>
       </c>
       <c r="M30" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="N30" s="1">
-        <v>1</v>
+        <v>0.98850185008074598</v>
       </c>
       <c r="O30" s="1">
-        <v>20.478277796150898</v>
+        <v>12.593272667303101</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -1724,46 +1724,46 @@
         <v>39</v>
       </c>
       <c r="B31" s="1">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.145595641895364</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.42857142857142799</v>
+      </c>
+      <c r="E31" s="1">
+        <v>155.39165950923299</v>
+      </c>
+      <c r="F31" s="1">
+        <v>7</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.96165638969144696</v>
+      </c>
+      <c r="H31" s="1">
+        <v>13.8982623401374</v>
+      </c>
+      <c r="I31" s="1">
         <v>0</v>
       </c>
-      <c r="C31" s="1">
-        <v>0.274300699300699</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1">
-        <v>156.72913180708201</v>
-      </c>
-      <c r="F31" s="1">
-        <v>8</v>
-      </c>
-      <c r="G31" s="1">
-        <v>0.983826603368543</v>
-      </c>
-      <c r="H31" s="1">
-        <v>13.6624611054794</v>
-      </c>
-      <c r="I31" s="1">
-        <v>1</v>
-      </c>
       <c r="J31" s="1">
-        <v>0</v>
+        <v>0.27744250130929099</v>
       </c>
       <c r="K31" s="1">
-        <v>2.4807692307692299</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="L31" s="1">
-        <v>204.122607052294</v>
+        <v>119.849562105299</v>
       </c>
       <c r="M31" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="N31" s="1">
-        <v>0.87125411257858598</v>
+        <v>0.98450732401859298</v>
       </c>
       <c r="O31" s="1">
-        <v>13.817059924286299</v>
+        <v>10.774435879605001</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -1771,46 +1771,46 @@
         <v>40</v>
       </c>
       <c r="B32" s="1">
-        <v>0</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="C32" s="1">
-        <v>0.152179691653375</v>
+        <v>5.6799819453847801E-2</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="E32" s="1">
-        <v>286.88210181884699</v>
+        <v>428.25042243963702</v>
       </c>
       <c r="F32" s="1">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G32" s="1">
-        <v>0.97712843766982904</v>
+        <v>0.98040486305110897</v>
       </c>
       <c r="H32" s="1">
-        <v>23.643830355335599</v>
+        <v>23.626768733143798</v>
       </c>
       <c r="I32" s="1">
-        <v>1</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="J32" s="1">
         <v>0</v>
       </c>
       <c r="K32" s="1">
-        <v>1.08421052631578</v>
+        <v>1</v>
       </c>
       <c r="L32" s="1">
-        <v>605.90855905240801</v>
+        <v>437.58522946951302</v>
       </c>
       <c r="M32" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N32" s="1">
-        <v>0.99825743817294499</v>
+        <v>0.99053365177401298</v>
       </c>
       <c r="O32" s="1">
-        <v>27.6424081740494</v>
+        <v>17.686325904142301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
previo vs criterio1 1000 soluciones
</commit_message>
<xml_diff>
--- a/Docs importantes/previoVSCriterio1.xlsx
+++ b/Docs importantes/previoVSCriterio1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Investigacion-maxima-diversidad\Docs importantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9279B6F-DB2F-433B-9CB9-71DEA868E714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CE29B2-828D-4D1E-B6A6-217D35EE0D41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{624528B1-719E-46FD-9C2E-53A661800D81}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
-    <t>GRASPConstructive_Criterion1_Seed_13_SolCount_250</t>
-  </si>
-  <si>
     <t>previo</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>IGD</t>
+  </si>
+  <si>
+    <t>GRASPConstructive_Criterion1_Seed_13_SolCount_100</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,30 +551,30 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1">
         <f>AVERAGE(B9:B32)</f>
@@ -607,7 +607,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
         <f>AVERAGE(I9:I32)</f>
@@ -630,7 +630,7 @@
         <v>92.333333333333329</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(N9:N32)</f>
         <v>0.97744691276959672</v>
       </c>
       <c r="H3" s="1">
@@ -640,54 +640,54 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>9</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>10</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>11</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>12</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>13</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>14</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>15</v>
-      </c>
-      <c r="O8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>0.35294117647058798</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
         <v>9.0909090909090898E-2</v>
@@ -828,7 +828,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
         <v>0.625</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>0.77272727272727204</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
         <v>0.57142857142857095</v>
@@ -969,7 +969,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1">
         <v>0.11111111111111099</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1">
         <v>0.68421052631578905</v>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1">
         <v>0.57142857142857095</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1">
         <v>0.58823529411764697</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1">
         <v>0.14285714285714199</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1">
         <v>0.88</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1">
         <v>0.78571428571428503</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1">
         <v>0.16666666666666599</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>0.66666666666666596</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1">
         <v>0.125</v>
@@ -1486,7 +1486,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1">
         <v>0.28571428571428498</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1">
         <v>0.16666666666666599</v>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="1">
         <v>0.31578947368421001</v>
@@ -1674,7 +1674,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1">
         <v>0.77777777777777701</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="1">
         <v>0.57142857142857095</v>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1">
         <v>0.33333333333333298</v>

</xml_diff>